<commit_message>
Simple timestamp of the output
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepe\Documents\Python Scrips\CSIC Scrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepe\Documents\Python Scrips\CSIC Scrapper\CSIC-Scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C074BFEC-A786-46F9-B142-52DD3B301C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D36242-F3F1-4337-8B93-53138DFB67C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$207</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1971,12 +1974,48 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2010,12 +2049,19 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2321,16 +2367,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91.42578125" customWidth="1"/>
-    <col min="3" max="3" width="71.140625" customWidth="1"/>
+    <col min="2" max="2" width="156.140625" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2345,11 +2392,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
@@ -2373,11 +2418,9 @@
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -2387,11 +2430,9 @@
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -2401,11 +2442,9 @@
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -2429,11 +2468,9 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
@@ -2443,11 +2480,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -2457,11 +2492,9 @@
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
@@ -2471,11 +2504,9 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
@@ -2485,11 +2516,9 @@
         <v>424</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
@@ -2499,11 +2528,9 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
@@ -2513,11 +2540,9 @@
         <v>426</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
@@ -2527,11 +2552,9 @@
         <v>427</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
@@ -2541,11 +2564,9 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
@@ -2555,11 +2576,9 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
@@ -2569,11 +2588,9 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
@@ -2583,11 +2600,9 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C19" t="s">
@@ -2597,11 +2612,9 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
@@ -2611,11 +2624,9 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
@@ -2625,11 +2636,9 @@
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
@@ -2639,11 +2648,9 @@
         <v>435</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
@@ -2653,11 +2660,9 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
@@ -2667,11 +2672,9 @@
         <v>437</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
@@ -2681,11 +2684,9 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
@@ -2695,11 +2696,9 @@
         <v>439</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
@@ -2709,11 +2708,9 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
@@ -2723,11 +2720,9 @@
         <v>441</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
@@ -2751,11 +2746,9 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
@@ -2765,11 +2758,9 @@
         <v>444</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C32" t="s">
@@ -2779,11 +2770,9 @@
         <v>445</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
@@ -2793,11 +2782,9 @@
         <v>446</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C34" t="s">
@@ -2835,11 +2822,9 @@
         <v>449</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C37" t="s">
@@ -2849,11 +2834,9 @@
         <v>450</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C38" t="s">
@@ -2863,10 +2846,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
       <c r="B39" t="s">
         <v>40</v>
       </c>
@@ -2881,7 +2862,7 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C40" t="s">
@@ -2891,11 +2872,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
@@ -2905,11 +2884,9 @@
         <v>454</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C42" t="s">
@@ -2919,11 +2896,9 @@
         <v>455</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C43" t="s">
@@ -2937,7 +2912,7 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C44" t="s">
@@ -2947,11 +2922,9 @@
         <v>457</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C45" t="s">
@@ -2961,11 +2934,9 @@
         <v>458</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C46" t="s">
@@ -2975,11 +2946,9 @@
         <v>459</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C47" t="s">
@@ -2989,11 +2958,9 @@
         <v>460</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C48" t="s">
@@ -3003,11 +2970,9 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C49" t="s">
@@ -3017,11 +2982,9 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C50" t="s">
@@ -3031,11 +2994,9 @@
         <v>463</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C51" t="s">
@@ -3049,7 +3010,7 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C52" t="s">
@@ -3059,11 +3020,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C53" t="s">
@@ -3073,11 +3032,9 @@
         <v>466</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C54" t="s">
@@ -3087,11 +3044,9 @@
         <v>467</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C55" t="s">
@@ -3101,11 +3056,9 @@
         <v>468</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C56" t="s">
@@ -3115,11 +3068,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C57" t="s">
@@ -3143,11 +3094,9 @@
         <v>471</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C59" t="s">
@@ -3157,11 +3106,9 @@
         <v>472</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C60" t="s">
@@ -3171,11 +3118,9 @@
         <v>473</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C61" t="s">
@@ -3189,7 +3134,7 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C62" t="s">
@@ -3199,11 +3144,9 @@
         <v>475</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C63" t="s">
@@ -3213,11 +3156,9 @@
         <v>476</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C64" t="s">
@@ -3227,11 +3168,9 @@
         <v>477</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C65" t="s">
@@ -3241,11 +3180,9 @@
         <v>478</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C66" t="s">
@@ -3255,11 +3192,9 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C67" t="s">
@@ -3269,11 +3204,9 @@
         <v>480</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C68" t="s">
@@ -3297,11 +3230,9 @@
         <v>482</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C70" t="s">
@@ -3325,11 +3256,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>70</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C72" t="s">
@@ -3339,11 +3268,9 @@
         <v>485</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>71</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C73" t="s">
@@ -3353,11 +3280,9 @@
         <v>486</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>72</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C74" t="s">
@@ -3381,11 +3306,9 @@
         <v>488</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C76" t="s">
@@ -3395,11 +3318,9 @@
         <v>489</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C77" t="s">
@@ -3409,11 +3330,9 @@
         <v>490</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>76</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C78" t="s">
@@ -3423,11 +3342,9 @@
         <v>491</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>77</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C79" t="s">
@@ -3451,11 +3368,9 @@
         <v>493</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>79</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C81" t="s">
@@ -3469,7 +3384,7 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C82" t="s">
@@ -3479,11 +3394,9 @@
         <v>495</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>81</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C83" t="s">
@@ -3493,11 +3406,9 @@
         <v>496</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>82</v>
-      </c>
-      <c r="B84" t="s">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C84" t="s">
@@ -3507,11 +3418,9 @@
         <v>497</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>83</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C85" t="s">
@@ -3521,11 +3430,9 @@
         <v>498</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>84</v>
-      </c>
-      <c r="B86" t="s">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C86" t="s">
@@ -3539,7 +3446,7 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C87" t="s">
@@ -3549,11 +3456,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>86</v>
-      </c>
-      <c r="B88" t="s">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C88" t="s">
@@ -3563,11 +3468,9 @@
         <v>501</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>87</v>
-      </c>
-      <c r="B89" t="s">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C89" t="s">
@@ -3581,7 +3484,7 @@
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C90" t="s">
@@ -3595,7 +3498,7 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C91" t="s">
@@ -3605,11 +3508,9 @@
         <v>504</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>90</v>
-      </c>
-      <c r="B92" t="s">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C92" t="s">
@@ -3619,11 +3520,9 @@
         <v>505</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>91</v>
-      </c>
-      <c r="B93" t="s">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C93" t="s">
@@ -3633,11 +3532,9 @@
         <v>506</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>92</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C94" t="s">
@@ -3651,7 +3548,7 @@
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C95" t="s">
@@ -3661,11 +3558,9 @@
         <v>508</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>94</v>
-      </c>
-      <c r="B96" t="s">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C96" t="s">
@@ -3675,11 +3570,9 @@
         <v>509</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>95</v>
-      </c>
-      <c r="B97" t="s">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C97" t="s">
@@ -3689,11 +3582,9 @@
         <v>510</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>96</v>
-      </c>
-      <c r="B98" t="s">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C98" t="s">
@@ -3703,11 +3594,9 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>97</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C99" t="s">
@@ -3717,11 +3606,9 @@
         <v>512</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>98</v>
-      </c>
-      <c r="B100" t="s">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C100" t="s">
@@ -3735,7 +3622,7 @@
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C101" t="s">
@@ -3745,11 +3632,9 @@
         <v>514</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>100</v>
-      </c>
-      <c r="B102" t="s">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C102" t="s">
@@ -3759,11 +3644,9 @@
         <v>515</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>101</v>
-      </c>
-      <c r="B103" t="s">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="3" t="s">
         <v>104</v>
       </c>
       <c r="C103" t="s">
@@ -3773,11 +3656,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>102</v>
-      </c>
-      <c r="B104" t="s">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C104" t="s">
@@ -3787,11 +3668,9 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>103</v>
-      </c>
-      <c r="B105" t="s">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C105" t="s">
@@ -3801,11 +3680,9 @@
         <v>518</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>104</v>
-      </c>
-      <c r="B106" t="s">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C106" t="s">
@@ -3815,11 +3692,9 @@
         <v>519</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>105</v>
-      </c>
-      <c r="B107" t="s">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C107" t="s">
@@ -3833,7 +3708,7 @@
       <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C108" t="s">
@@ -3843,11 +3718,9 @@
         <v>521</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>107</v>
-      </c>
-      <c r="B109" t="s">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C109" t="s">
@@ -3857,11 +3730,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>108</v>
-      </c>
-      <c r="B110" t="s">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C110" t="s">
@@ -3871,11 +3742,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>109</v>
-      </c>
-      <c r="B111" t="s">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="B111" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C111" t="s">
@@ -3885,11 +3754,9 @@
         <v>524</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>110</v>
-      </c>
-      <c r="B112" t="s">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C112" t="s">
@@ -3899,11 +3766,9 @@
         <v>525</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>111</v>
-      </c>
-      <c r="B113" t="s">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C113" t="s">
@@ -3917,7 +3782,7 @@
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C114" t="s">
@@ -3931,7 +3796,7 @@
       <c r="A115" s="1">
         <v>113</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="7" t="s">
         <v>116</v>
       </c>
       <c r="C115" t="s">
@@ -3941,11 +3806,9 @@
         <v>528</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>114</v>
-      </c>
-      <c r="B116" t="s">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C116" t="s">
@@ -3955,11 +3818,9 @@
         <v>529</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>115</v>
-      </c>
-      <c r="B117" t="s">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C117" t="s">
@@ -3969,11 +3830,9 @@
         <v>530</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>116</v>
-      </c>
-      <c r="B118" t="s">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C118" t="s">
@@ -3983,11 +3842,9 @@
         <v>531</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119" t="s">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C119" t="s">
@@ -3997,11 +3854,9 @@
         <v>532</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>118</v>
-      </c>
-      <c r="B120" t="s">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C120" t="s">
@@ -4011,11 +3866,9 @@
         <v>533</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>119</v>
-      </c>
-      <c r="B121" t="s">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C121" t="s">
@@ -4025,11 +3878,9 @@
         <v>534</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>120</v>
-      </c>
-      <c r="B122" t="s">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C122" t="s">
@@ -4043,7 +3894,7 @@
       <c r="A123" s="1">
         <v>121</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="9" t="s">
         <v>124</v>
       </c>
       <c r="C123" t="s">
@@ -4053,11 +3904,9 @@
         <v>536</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>122</v>
-      </c>
-      <c r="B124" t="s">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C124" t="s">
@@ -4067,11 +3916,9 @@
         <v>537</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>123</v>
-      </c>
-      <c r="B125" t="s">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C125" t="s">
@@ -4081,11 +3928,9 @@
         <v>538</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>124</v>
-      </c>
-      <c r="B126" t="s">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C126" t="s">
@@ -4123,11 +3968,9 @@
         <v>541</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>127</v>
-      </c>
-      <c r="B129" t="s">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+      <c r="B129" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C129" t="s">
@@ -4137,11 +3980,9 @@
         <v>542</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>128</v>
-      </c>
-      <c r="B130" t="s">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C130" t="s">
@@ -4151,11 +3992,9 @@
         <v>543</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>129</v>
-      </c>
-      <c r="B131" t="s">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C131" t="s">
@@ -4169,7 +4008,7 @@
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C132" t="s">
@@ -4179,11 +4018,9 @@
         <v>545</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>131</v>
-      </c>
-      <c r="B133" t="s">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C133" t="s">
@@ -4193,11 +4030,9 @@
         <v>546</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134" t="s">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="3" t="s">
         <v>135</v>
       </c>
       <c r="C134" t="s">
@@ -4207,11 +4042,9 @@
         <v>547</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135" t="s">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="3" t="s">
         <v>136</v>
       </c>
       <c r="C135" t="s">
@@ -4235,11 +4068,9 @@
         <v>549</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137" t="s">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="3" t="s">
         <v>138</v>
       </c>
       <c r="C137" t="s">
@@ -4249,11 +4080,9 @@
         <v>550</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <v>136</v>
-      </c>
-      <c r="B138" t="s">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C138" t="s">
@@ -4263,11 +4092,9 @@
         <v>551</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139" t="s">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C139" t="s">
@@ -4277,11 +4104,9 @@
         <v>552</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140" t="s">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="3" t="s">
         <v>141</v>
       </c>
       <c r="C140" t="s">
@@ -4291,11 +4116,9 @@
         <v>553</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141" t="s">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C141" t="s">
@@ -4309,7 +4132,7 @@
       <c r="A142" s="1">
         <v>140</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="7" t="s">
         <v>143</v>
       </c>
       <c r="C142" t="s">
@@ -4319,11 +4142,9 @@
         <v>555</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143" t="s">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C143" t="s">
@@ -4333,11 +4154,9 @@
         <v>556</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144" t="s">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="3" t="s">
         <v>145</v>
       </c>
       <c r="C144" t="s">
@@ -4347,11 +4166,9 @@
         <v>557</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145" t="s">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="3" t="s">
         <v>146</v>
       </c>
       <c r="C145" t="s">
@@ -4361,11 +4178,9 @@
         <v>558</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>144</v>
-      </c>
-      <c r="B146" t="s">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C146" t="s">
@@ -4375,11 +4190,9 @@
         <v>559</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>145</v>
-      </c>
-      <c r="B147" t="s">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C147" t="s">
@@ -4393,7 +4206,7 @@
       <c r="A148" s="1">
         <v>146</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="6" t="s">
         <v>149</v>
       </c>
       <c r="C148" t="s">
@@ -4403,11 +4216,9 @@
         <v>561</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149" t="s">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="3" t="s">
         <v>150</v>
       </c>
       <c r="C149" t="s">
@@ -4417,11 +4228,9 @@
         <v>562</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150" t="s">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+      <c r="B150" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C150" t="s">
@@ -4445,11 +4254,9 @@
         <v>564</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
-        <v>150</v>
-      </c>
-      <c r="B152" t="s">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+      <c r="B152" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C152" t="s">
@@ -4463,7 +4270,7 @@
       <c r="A153" s="1">
         <v>151</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="3" t="s">
         <v>154</v>
       </c>
       <c r="C153" t="s">
@@ -4473,11 +4280,9 @@
         <v>566</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>152</v>
-      </c>
-      <c r="B154" t="s">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+      <c r="B154" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C154" t="s">
@@ -4487,11 +4292,9 @@
         <v>567</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>153</v>
-      </c>
-      <c r="B155" t="s">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+      <c r="B155" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C155" t="s">
@@ -4501,11 +4304,9 @@
         <v>568</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>154</v>
-      </c>
-      <c r="B156" t="s">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+      <c r="B156" s="3" t="s">
         <v>157</v>
       </c>
       <c r="C156" t="s">
@@ -4515,11 +4316,9 @@
         <v>569</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <v>155</v>
-      </c>
-      <c r="B157" t="s">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+      <c r="B157" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C157" t="s">
@@ -4529,11 +4328,9 @@
         <v>570</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>156</v>
-      </c>
-      <c r="B158" t="s">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+      <c r="B158" s="3" t="s">
         <v>159</v>
       </c>
       <c r="C158" t="s">
@@ -4543,11 +4340,9 @@
         <v>571</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>157</v>
-      </c>
-      <c r="B159" t="s">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1"/>
+      <c r="B159" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C159" t="s">
@@ -4557,11 +4352,9 @@
         <v>572</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>158</v>
-      </c>
-      <c r="B160" t="s">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1"/>
+      <c r="B160" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C160" t="s">
@@ -4571,11 +4364,9 @@
         <v>573</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>159</v>
-      </c>
-      <c r="B161" t="s">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+      <c r="B161" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C161" t="s">
@@ -4585,11 +4376,9 @@
         <v>574</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>160</v>
-      </c>
-      <c r="B162" t="s">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+      <c r="B162" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C162" t="s">
@@ -4599,11 +4388,9 @@
         <v>575</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <v>161</v>
-      </c>
-      <c r="B163" t="s">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+      <c r="B163" s="3" t="s">
         <v>164</v>
       </c>
       <c r="C163" t="s">
@@ -4613,11 +4400,9 @@
         <v>576</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <v>162</v>
-      </c>
-      <c r="B164" t="s">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+      <c r="B164" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C164" t="s">
@@ -4627,11 +4412,9 @@
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
-        <v>163</v>
-      </c>
-      <c r="B165" t="s">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1"/>
+      <c r="B165" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C165" t="s">
@@ -4641,11 +4424,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
-        <v>164</v>
-      </c>
-      <c r="B166" t="s">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1"/>
+      <c r="B166" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C166" t="s">
@@ -4655,11 +4436,9 @@
         <v>579</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>165</v>
-      </c>
-      <c r="B167" t="s">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+      <c r="B167" s="3" t="s">
         <v>168</v>
       </c>
       <c r="C167" t="s">
@@ -4669,11 +4448,9 @@
         <v>580</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
-        <v>166</v>
-      </c>
-      <c r="B168" t="s">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1"/>
+      <c r="B168" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C168" t="s">
@@ -4683,11 +4460,9 @@
         <v>581</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>167</v>
-      </c>
-      <c r="B169" t="s">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1"/>
+      <c r="B169" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C169" t="s">
@@ -4697,11 +4472,9 @@
         <v>582</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>168</v>
-      </c>
-      <c r="B170" t="s">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+      <c r="B170" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C170" t="s">
@@ -4711,11 +4484,9 @@
         <v>583</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
-        <v>169</v>
-      </c>
-      <c r="B171" t="s">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+      <c r="B171" s="3" t="s">
         <v>172</v>
       </c>
       <c r="C171" t="s">
@@ -4725,11 +4496,9 @@
         <v>584</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
-        <v>170</v>
-      </c>
-      <c r="B172" t="s">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1"/>
+      <c r="B172" s="3" t="s">
         <v>173</v>
       </c>
       <c r="C172" t="s">
@@ -4739,11 +4508,9 @@
         <v>585</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
-        <v>171</v>
-      </c>
-      <c r="B173" t="s">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+      <c r="B173" s="3" t="s">
         <v>174</v>
       </c>
       <c r="C173" t="s">
@@ -4753,11 +4520,9 @@
         <v>586</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
-        <v>172</v>
-      </c>
-      <c r="B174" t="s">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+      <c r="B174" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C174" t="s">
@@ -4767,11 +4532,9 @@
         <v>587</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
-        <v>173</v>
-      </c>
-      <c r="B175" t="s">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+      <c r="B175" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C175" t="s">
@@ -4781,11 +4544,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
-        <v>174</v>
-      </c>
-      <c r="B176" t="s">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+      <c r="B176" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C176" t="s">
@@ -4795,11 +4556,9 @@
         <v>589</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
-        <v>175</v>
-      </c>
-      <c r="B177" t="s">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+      <c r="B177" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C177" t="s">
@@ -4809,11 +4568,9 @@
         <v>590</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
-        <v>176</v>
-      </c>
-      <c r="B178" t="s">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C178" t="s">
@@ -4823,11 +4580,9 @@
         <v>591</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
-        <v>177</v>
-      </c>
-      <c r="B179" t="s">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+      <c r="B179" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C179" t="s">
@@ -4837,11 +4592,9 @@
         <v>592</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
-        <v>178</v>
-      </c>
-      <c r="B180" t="s">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C180" t="s">
@@ -4865,11 +4618,9 @@
         <v>594</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
-        <v>180</v>
-      </c>
-      <c r="B182" t="s">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1"/>
+      <c r="B182" s="3" t="s">
         <v>183</v>
       </c>
       <c r="C182" t="s">
@@ -4879,11 +4630,9 @@
         <v>595</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>181</v>
-      </c>
-      <c r="B183" t="s">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1"/>
+      <c r="B183" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C183" t="s">
@@ -4893,11 +4642,9 @@
         <v>596</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
-        <v>182</v>
-      </c>
-      <c r="B184" t="s">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+      <c r="B184" s="3" t="s">
         <v>185</v>
       </c>
       <c r="C184" t="s">
@@ -4907,11 +4654,9 @@
         <v>597</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
-        <v>183</v>
-      </c>
-      <c r="B185" t="s">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+      <c r="B185" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C185" t="s">
@@ -4921,11 +4666,9 @@
         <v>598</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
-        <v>184</v>
-      </c>
-      <c r="B186" t="s">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+      <c r="B186" s="3" t="s">
         <v>187</v>
       </c>
       <c r="C186" t="s">
@@ -4935,11 +4678,9 @@
         <v>599</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
-        <v>185</v>
-      </c>
-      <c r="B187" t="s">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1"/>
+      <c r="B187" s="3" t="s">
         <v>188</v>
       </c>
       <c r="C187" t="s">
@@ -4949,11 +4690,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
-        <v>186</v>
-      </c>
-      <c r="B188" t="s">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1"/>
+      <c r="B188" s="3" t="s">
         <v>189</v>
       </c>
       <c r="C188" t="s">
@@ -4963,11 +4702,9 @@
         <v>601</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
-        <v>187</v>
-      </c>
-      <c r="B189" t="s">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1"/>
+      <c r="B189" s="3" t="s">
         <v>190</v>
       </c>
       <c r="C189" t="s">
@@ -4977,11 +4714,9 @@
         <v>602</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
-        <v>188</v>
-      </c>
-      <c r="B190" t="s">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1"/>
+      <c r="B190" s="3" t="s">
         <v>191</v>
       </c>
       <c r="C190" t="s">
@@ -4991,11 +4726,9 @@
         <v>603</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
-        <v>189</v>
-      </c>
-      <c r="B191" t="s">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1"/>
+      <c r="B191" s="3" t="s">
         <v>192</v>
       </c>
       <c r="C191" t="s">
@@ -5005,11 +4738,9 @@
         <v>604</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
-        <v>190</v>
-      </c>
-      <c r="B192" t="s">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1"/>
+      <c r="B192" s="3" t="s">
         <v>193</v>
       </c>
       <c r="C192" t="s">
@@ -5019,11 +4750,9 @@
         <v>605</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
-        <v>191</v>
-      </c>
-      <c r="B193" t="s">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1"/>
+      <c r="B193" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C193" t="s">
@@ -5033,11 +4762,9 @@
         <v>606</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
-        <v>192</v>
-      </c>
-      <c r="B194" t="s">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1"/>
+      <c r="B194" s="3" t="s">
         <v>195</v>
       </c>
       <c r="C194" t="s">
@@ -5051,7 +4778,7 @@
       <c r="A195" s="1">
         <v>193</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="8" t="s">
         <v>196</v>
       </c>
       <c r="C195" t="s">
@@ -5061,11 +4788,9 @@
         <v>608</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
-        <v>194</v>
-      </c>
-      <c r="B196" t="s">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1"/>
+      <c r="B196" s="3" t="s">
         <v>197</v>
       </c>
       <c r="C196" t="s">
@@ -5075,11 +4800,9 @@
         <v>609</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
-        <v>195</v>
-      </c>
-      <c r="B197" t="s">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1"/>
+      <c r="B197" s="3" t="s">
         <v>198</v>
       </c>
       <c r="C197" t="s">
@@ -5089,11 +4812,9 @@
         <v>610</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
-        <v>196</v>
-      </c>
-      <c r="B198" t="s">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+      <c r="B198" s="3" t="s">
         <v>199</v>
       </c>
       <c r="C198" t="s">
@@ -5103,11 +4824,9 @@
         <v>611</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
-        <v>197</v>
-      </c>
-      <c r="B199" t="s">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1"/>
+      <c r="B199" s="3" t="s">
         <v>200</v>
       </c>
       <c r="C199" t="s">
@@ -5117,11 +4836,9 @@
         <v>612</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
-        <v>198</v>
-      </c>
-      <c r="B200" t="s">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+      <c r="B200" s="3" t="s">
         <v>201</v>
       </c>
       <c r="C200" t="s">
@@ -5131,11 +4848,9 @@
         <v>613</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
-        <v>199</v>
-      </c>
-      <c r="B201" t="s">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+      <c r="B201" s="3" t="s">
         <v>202</v>
       </c>
       <c r="C201" t="s">
@@ -5145,11 +4860,9 @@
         <v>614</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
-        <v>200</v>
-      </c>
-      <c r="B202" t="s">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+      <c r="B202" s="3" t="s">
         <v>203</v>
       </c>
       <c r="C202" t="s">
@@ -5159,11 +4872,9 @@
         <v>615</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
-        <v>201</v>
-      </c>
-      <c r="B203" t="s">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1"/>
+      <c r="B203" s="3" t="s">
         <v>204</v>
       </c>
       <c r="C203" t="s">
@@ -5173,11 +4884,9 @@
         <v>616</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
-        <v>202</v>
-      </c>
-      <c r="B204" t="s">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+      <c r="B204" s="3" t="s">
         <v>205</v>
       </c>
       <c r="C204" t="s">
@@ -5187,11 +4896,9 @@
         <v>617</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
-        <v>203</v>
-      </c>
-      <c r="B205" t="s">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+      <c r="B205" s="3" t="s">
         <v>206</v>
       </c>
       <c r="C205" t="s">
@@ -5201,11 +4908,9 @@
         <v>618</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
-        <v>204</v>
-      </c>
-      <c r="B206" t="s">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+      <c r="B206" s="3" t="s">
         <v>207</v>
       </c>
       <c r="C206" t="s">
@@ -5215,11 +4920,9 @@
         <v>619</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
-        <v>205</v>
-      </c>
-      <c r="B207" t="s">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1"/>
+      <c r="B207" s="3" t="s">
         <v>208</v>
       </c>
       <c r="C207" t="s">
@@ -5230,6 +4933,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D207" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -5439,5 +5149,6 @@
     <hyperlink ref="D207" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId207"/>
 </worksheet>
 </file>
</xml_diff>